<commit_message>
141 Assemble Ship Detail
</commit_message>
<xml_diff>
--- a/GameMaster/RPGTale/Data/Data_Excel/AssembleMetaData.xlsx
+++ b/GameMaster/RPGTale/Data/Data_Excel/AssembleMetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\建造工程\Project\GameMaster\RPGTale\Data\Data_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4990EA-40C6-47A3-9710-FC3AFFA1E180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1491A6-E479-4614-ACC9-5E961DE00135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="2220" windowWidth="23205" windowHeight="12255" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="1575" windowWidth="23205" windowHeight="12255" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AssembleWarship" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>WarShipID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,6 +214,38 @@
   </si>
   <si>
     <t>Objects/Assemble/Ship/Ship001/Ship001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpriteOutput/Assemble/Icon/Assemble_Part_Engine_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PartIconSmall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpriteOutput/Assemble/Icon/Assemble_Part_Engine_Icon_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PartSprite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Warship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AssembleType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WarShip</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -632,29 +664,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -662,118 +696,127 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1">
         <v>100</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>500</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>5000</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>1.6</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>5.5</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>6</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1">
         <v>100</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>600</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>6000</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>5</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>1.5</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>8</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>15</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -789,7 +832,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -799,14 +842,14 @@
     <col min="3" max="3" width="58.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -843,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F246614B-2A30-4206-B3F6-1468D348947F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -891,22 +934,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA90FB13-0B57-4FEC-8B6D-736F2940F7EF}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -914,16 +960,25 @@
         <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -931,12 +986,21 @@
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>